<commit_message>
Sistema de Cadastro Python
</commit_message>
<xml_diff>
--- a/Usuarios_Planilha.xlsx
+++ b/Usuarios_Planilha.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,9 +431,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
@@ -520,6 +520,44 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Marineia</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Almeida</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>marineia123@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>12345678917</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>Aa123456789*</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: adiciona um campo para o admin apagar ou visualizar os dados do banco
</commit_message>
<xml_diff>
--- a/Usuarios_Planilha.xlsx
+++ b/Usuarios_Planilha.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,9 +431,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
     <col width="11" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
@@ -488,25 +488,25 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>Exemplo</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Soares</t>
+          <t>Teste</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>thiago@gmail.com</t>
+          <t>exemplo@gmail.com</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
@@ -515,196 +515,6 @@
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>Aa123456789*</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Julia</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Souza</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Julia@gmail.com</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>12345678917</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>Aa123456789*</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>João Pedro</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Costa da Silva</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>joao@gmail.com</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>53</v>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>01234567891</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="inlineStr">
-        <is>
-          <t>Aa123456789*</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Maria Eduarda</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>da Silva Peixoto</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>maria@gmail.com</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>82</v>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
-      </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>01234567890</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="inlineStr">
-        <is>
-          <t>Aa123456789*</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Lucas</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>alme</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>sdg@.</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>120</v>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>12301231548</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>Aasfdsdgdj1*</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>Joao Pedro</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>Santos Costa</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>gfgn@dingf.com</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="G7" s="2" t="inlineStr">
-        <is>
-          <t>12345678915</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="inlineStr">
         <is>
           <t>Aa123456789*</t>
         </is>

</xml_diff>